<commit_message>
Bug Fix Failed Input/Edit
</commit_message>
<xml_diff>
--- a/public/Template_Import_emodule.xlsx
+++ b/public/Template_Import_emodule.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Inaco\emodule\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA2CA6C6-04F3-4B82-8794-E4A831B88282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D181F88-1EE4-44D8-B8EB-7434EA546ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3816" yWindow="3360" windowWidth="17280" windowHeight="8880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,9 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>No.</t>
-  </si>
-  <si>
     <t>Title</t>
   </si>
   <si>
@@ -38,13 +35,16 @@
   </si>
   <si>
     <t>Sub-category</t>
+  </si>
+  <si>
+    <t>Video</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -90,10 +90,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -114,9 +113,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -154,7 +153,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -260,7 +259,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -402,7 +401,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -410,30 +409,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="2" max="2" width="16.21875" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" customWidth="1"/>
-    <col min="5" max="5" width="21.109375" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" customWidth="1"/>
+    <col min="4" max="4" width="21.109375" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -442,87 +441,38 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
-      <c r="B2" s="3"/>
-    </row>
-    <row r="3" spans="1:6">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
-      <c r="B3" s="3"/>
-    </row>
-    <row r="4" spans="1:6">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
-      <c r="B4" s="3"/>
-    </row>
-    <row r="5" spans="1:6">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
-      <c r="B5" s="3"/>
-    </row>
-    <row r="6" spans="1:6">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
-      <c r="B6" s="3"/>
-    </row>
-    <row r="7" spans="1:6">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
-      <c r="B7" s="3"/>
-    </row>
-    <row r="8" spans="1:6">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="3"/>
-    </row>
-    <row r="9" spans="1:6">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
-      <c r="B9" s="3"/>
-    </row>
-    <row r="10" spans="1:6">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
-      <c r="B10" s="3"/>
-    </row>
-    <row r="11" spans="1:6">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
-      <c r="B11" s="3"/>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="2"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="2"/>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="2"/>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="2"/>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="2"/>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="2"/>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="2"/>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="2"/>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="2"/>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="2"/>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" s="2"/>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" s="2"/>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>